<commit_message>
Forms A e B
</commit_message>
<xml_diff>
--- a/outputs/expansao_formA.xlsx
+++ b/outputs/expansao_formA.xlsx
@@ -468,44 +468,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="32" customWidth="1" min="3" max="3"/>
-    <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Município</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>UVR</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Quem preencheu</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Responsável</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Situação</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Data de Envio</t>
         </is>
@@ -514,25 +522,30 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Alto Paraná</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -541,25 +554,30 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Amaporã</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -568,25 +586,30 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
           <t>Apucarana</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -595,25 +618,30 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
           <t>Atalaia</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -622,25 +650,30 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
           <t>Barracão</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -649,25 +682,30 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
           <t>Borrazópolis</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -676,25 +714,30 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
           <t>Cambará</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -703,25 +746,30 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
           <t>Campina da Lagoa</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>30/07/2025</t>
         </is>
@@ -730,25 +778,30 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
           <t>Campo Largo</t>
         </is>
       </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>20/06/2025</t>
         </is>
@@ -757,25 +810,30 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
           <t>Campo Largo</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>20/06/2025</t>
         </is>
@@ -784,25 +842,30 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
           <t>Campo Largo</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>20/06/2025</t>
         </is>
@@ -811,25 +874,30 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
           <t>Campo Largo</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="D13" s="2" t="inlineStr">
         <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D13" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>20/06/2025</t>
         </is>
@@ -838,25 +906,30 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
           <t>Campo Largo</t>
         </is>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
         <is>
           <t>20/06/2025</t>
         </is>
@@ -865,25 +938,30 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
           <t>Campo Magro</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -892,25 +970,30 @@
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
           <t>Capanema</t>
         </is>
       </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="inlineStr">
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -919,25 +1002,30 @@
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
           <t>Cerro Azul</t>
         </is>
       </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="inlineStr">
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -946,25 +1034,30 @@
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
           <t>Colorado</t>
         </is>
       </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D18" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
+      <c r="E18" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -973,25 +1066,30 @@
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
           <t>Coronel Vivida</t>
         </is>
       </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
           <t>Tatiane Lordeiro de Andrade</t>
         </is>
       </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E19" s="2" t="inlineStr">
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
         <is>
           <t>24/06/2025</t>
         </is>
@@ -1000,25 +1098,30 @@
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
           <t>Cruzeiro do Sul</t>
         </is>
       </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E20" s="2" t="inlineStr">
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1027,25 +1130,30 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
           <t>Enéas Marques</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -1054,25 +1162,30 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
           <t>Francisco Beltrão</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E22" s="2" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t>04/07/2025</t>
         </is>
@@ -1081,25 +1194,30 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
           <t>Francisco Beltrão</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E23" s="2" t="inlineStr">
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>04/07/2025</t>
         </is>
@@ -1108,25 +1226,30 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
           <t>Francisco Beltrão</t>
         </is>
       </c>
-      <c r="B24" s="2" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C24" s="2" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E24" s="2" t="inlineStr">
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
         <is>
           <t>04/07/2025</t>
         </is>
@@ -1135,25 +1258,30 @@
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
           <t>General Carneiro</t>
         </is>
       </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
           <t>Tatiane Lordeiro de Andrade</t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E25" s="2" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
         <is>
           <t>24/06/2025</t>
         </is>
@@ -1162,25 +1290,30 @@
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
           <t>Ibaiti</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E26" s="2" t="inlineStr">
+      <c r="E26" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1189,25 +1322,30 @@
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
           <t>Jaguapitã</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D27" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E27" s="2" t="inlineStr">
+      <c r="E27" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1216,25 +1354,30 @@
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
           <t>Jaguariaíva</t>
         </is>
       </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D28" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E28" s="2" t="inlineStr">
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1243,25 +1386,30 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
           <t>Jardim Alegre</t>
         </is>
       </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D29" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E29" s="2" t="inlineStr">
+      <c r="E29" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1270,25 +1418,30 @@
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
           <t>Kaloré</t>
         </is>
       </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="inlineStr">
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1297,25 +1450,30 @@
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
           <t>Lapa</t>
         </is>
       </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D31" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E31" s="2" t="inlineStr">
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1324,25 +1482,30 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
           <t>Laranjeiras do Sul</t>
         </is>
       </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
           <t>Juliana Elisabete Correia</t>
         </is>
       </c>
-      <c r="D32" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E32" s="2" t="inlineStr">
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -1351,25 +1514,30 @@
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
           <t>Mandaguaçu</t>
         </is>
       </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C33" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="inlineStr">
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1378,25 +1546,30 @@
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
           <t>Mandaguari</t>
         </is>
       </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D34" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E34" s="2" t="inlineStr">
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1405,25 +1578,30 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
           <t>Marmeleiro</t>
         </is>
       </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D35" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="inlineStr">
+      <c r="E35" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1432,25 +1610,30 @@
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
           <t>Mato Rico</t>
         </is>
       </c>
-      <c r="B36" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
           <t>Juliana Elisabete Correia</t>
         </is>
       </c>
-      <c r="D36" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E36" s="2" t="inlineStr">
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
         <is>
           <t>05/06/2025</t>
         </is>
@@ -1459,25 +1642,30 @@
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="inlineStr">
+        <is>
           <t>Nova Tebas</t>
         </is>
       </c>
-      <c r="B37" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D37" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E37" s="2" t="inlineStr">
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
         <is>
           <t>30/07/2025</t>
         </is>
@@ -1486,25 +1674,30 @@
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
           <t>Ortigueira</t>
         </is>
       </c>
-      <c r="B38" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D38" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E38" s="2" t="inlineStr">
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1513,25 +1706,30 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="inlineStr">
+        <is>
           <t>Palmital</t>
         </is>
       </c>
-      <c r="B39" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
           <t>Tatiane Lordeiro de Andrade</t>
         </is>
       </c>
-      <c r="D39" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E39" s="2" t="inlineStr">
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
         <is>
           <t>24/06/2025</t>
         </is>
@@ -1540,25 +1738,30 @@
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
           <t>Paraíso do Norte</t>
         </is>
       </c>
-      <c r="B40" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E40" s="2" t="inlineStr">
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1567,25 +1770,30 @@
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="inlineStr">
+        <is>
           <t>Presidente Castelo Branco</t>
         </is>
       </c>
-      <c r="B41" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
           <t>Diana Pivatto</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E41" s="2" t="inlineStr">
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1594,25 +1802,30 @@
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
           <t>Quedas do Iguaçu</t>
         </is>
       </c>
-      <c r="B42" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
           <t>Tatiane Lordeiro de Andrade</t>
         </is>
       </c>
-      <c r="D42" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E42" s="2" t="inlineStr">
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1621,25 +1834,30 @@
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
           <t>Realeza</t>
         </is>
       </c>
-      <c r="B43" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C43" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D43" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E43" s="2" t="inlineStr">
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1648,25 +1866,30 @@
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
           <t>Reserva do Iguaçu</t>
         </is>
       </c>
-      <c r="B44" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
           <t>Juliana Elisabete Correia</t>
         </is>
       </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E44" s="2" t="inlineStr">
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -1675,25 +1898,30 @@
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="inlineStr">
+        <is>
           <t>Ribeirão Claro</t>
         </is>
       </c>
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C45" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E45" s="2" t="inlineStr">
+      <c r="E45" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1702,25 +1930,30 @@
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
           <t>Rio Branco do Sul</t>
         </is>
       </c>
-      <c r="B46" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E46" s="2" t="inlineStr">
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1729,25 +1962,30 @@
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
           <t>Rio Branco do Sul</t>
         </is>
       </c>
-      <c r="B47" s="2" t="inlineStr">
+      <c r="C47" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="C47" s="2" t="inlineStr">
-        <is>
-          <t>---</t>
-        </is>
-      </c>
-      <c r="D47" s="4" t="inlineStr">
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="inlineStr">
         <is>
           <t>Não Enviado</t>
         </is>
       </c>
-      <c r="E47" s="2" t="inlineStr">
+      <c r="F47" s="2" t="inlineStr">
         <is>
           <t>---</t>
         </is>
@@ -1756,25 +1994,30 @@
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
           <t>Rio Negro</t>
         </is>
       </c>
-      <c r="B48" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E48" s="2" t="inlineStr">
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
         <is>
           <t>21/05/2025</t>
         </is>
@@ -1783,25 +2026,30 @@
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
           <t>Salgado Filho</t>
         </is>
       </c>
-      <c r="B49" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C49" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
           <t>Vanessa Kaupka</t>
         </is>
       </c>
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E49" s="2" t="inlineStr">
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -1810,25 +2058,30 @@
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
           <t>Santa Maria do Oeste</t>
         </is>
       </c>
-      <c r="B50" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
           <t>Juliana Elisabete Correia</t>
         </is>
       </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E50" s="2" t="inlineStr">
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
         <is>
           <t>10/04/2025</t>
         </is>
@@ -1837,25 +2090,30 @@
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
           <t>Santa Mariana</t>
         </is>
       </c>
-      <c r="B51" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C51" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E51" s="2" t="inlineStr">
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1864,25 +2122,30 @@
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
           <t>Santa Mônica</t>
         </is>
       </c>
-      <c r="B52" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E52" s="2" t="inlineStr">
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1891,25 +2154,30 @@
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
+        <is>
           <t>Santana do Itararé</t>
         </is>
       </c>
-      <c r="B53" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C53" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
           <t>Johvanny Lourenço Mendonça</t>
         </is>
       </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E53" s="2" t="inlineStr">
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
         <is>
           <t>03/06/2025</t>
         </is>
@@ -1918,25 +2186,30 @@
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
           <t>São João</t>
         </is>
       </c>
-      <c r="B54" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
           <t>Tatiane Lordeiro de Andrade</t>
         </is>
       </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E54" s="2" t="inlineStr">
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
         <is>
           <t>24/06/2025</t>
         </is>
@@ -1945,25 +2218,30 @@
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
           <t>São João do Caiuá</t>
         </is>
       </c>
-      <c r="B55" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C55" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
           <t>Mario Ricardo Guadagnin</t>
         </is>
       </c>
-      <c r="D55" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E55" s="2" t="inlineStr">
+      <c r="E55" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -1972,25 +2250,30 @@
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
           <t>São João do Ivaí</t>
         </is>
       </c>
-      <c r="B56" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>---</t>
-        </is>
-      </c>
-      <c r="D56" s="4" t="inlineStr">
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
         <is>
           <t>Não Enviado</t>
         </is>
       </c>
-      <c r="E56" s="2" t="inlineStr">
+      <c r="F56" s="2" t="inlineStr">
         <is>
           <t>---</t>
         </is>
@@ -1999,25 +2282,30 @@
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="inlineStr">
+        <is>
           <t>São João do Triunfo</t>
         </is>
       </c>
-      <c r="B57" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C57" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E57" s="2" t="inlineStr">
+      <c r="E57" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -2026,25 +2314,30 @@
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
           <t>Tijucas do Sul</t>
         </is>
       </c>
-      <c r="B58" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
           <t>Kelly Ronsani de Barros</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="E58" s="2" t="inlineStr">
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
         <is>
           <t>04/06/2025</t>
         </is>
@@ -2052,7 +2345,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57 E58" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Enviado,Não Enviado"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>